<commit_message>
updating viz tables to fit correct data
Updated loa to include all analysis.
For each level, it will filter the results accordingly.
Wriggling around naming to fit the wide and gt table.
</commit_message>
<xml_diff>
--- a/input_tool/edu_analysistools_loa.xlsx
+++ b/input_tool/edu_analysistools_loa.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann SAY\Desktop\git\humind\EduAnalysisTool\input_tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann SAY\Desktop\git\EduAnalysisTool\input_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8E0571-68B5-40EF-ADF5-61267F9EFBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7276E6A8-92F6-4252-B86D-19E267DE1BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{172E695D-8722-4AF3-920F-94814F3A8B09}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{172E695D-8722-4AF3-920F-94814F3A8B09}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$85</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="54">
   <si>
     <t>analysis_var</t>
   </si>
@@ -155,6 +155,12 @@
     <t>edu_ind_no_access_d</t>
   </si>
   <si>
+    <t>pop_group</t>
+  </si>
+  <si>
+    <t>pop_group, ind_gender</t>
+  </si>
+  <si>
     <t>overall</t>
   </si>
   <si>
@@ -185,10 +191,16 @@
     <t>% of children accessing another type of education?</t>
   </si>
   <si>
-    <t>setting</t>
-  </si>
-  <si>
-    <t>setting, ind_gender</t>
+    <t>edu_school_cycle_d, pop_group</t>
+  </si>
+  <si>
+    <t>edu_school_cycle_d, pop_group, ind_gender</t>
+  </si>
+  <si>
+    <t>edu_school_cycle_d,pop_group</t>
+  </si>
+  <si>
+    <t>edu_school_cycle_d,pop_group, ind_gender</t>
   </si>
 </sst>
 </file>
@@ -1028,11 +1040,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549ABC9E-401F-4507-8765-75A12C3B174F}">
-  <dimension ref="A1:K83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE1FF5D-95CC-49D0-8C54-8D9CF98199B7}">
+  <dimension ref="A1:K85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,13 +1068,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -1074,7 +1086,7 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1088,7 +1100,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1097,16 +1109,16 @@
         <v>0</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
@@ -1123,7 +1135,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -1158,7 +1170,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1193,7 +1205,7 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -1228,7 +1240,7 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -1263,7 +1275,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -1298,7 +1310,7 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -1333,7 +1345,7 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -1368,7 +1380,7 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -1403,7 +1415,7 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -1447,16 +1459,16 @@
         <v>0</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="b">
         <v>0</v>
@@ -1622,16 +1634,16 @@
         <v>0</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="b">
         <v>0</v>
@@ -1788,7 +1800,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
@@ -1823,7 +1835,7 @@
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
@@ -1858,7 +1870,7 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
@@ -1893,7 +1905,7 @@
         <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -1928,7 +1940,7 @@
         <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -1963,7 +1975,7 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
@@ -1998,7 +2010,7 @@
         <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -2033,7 +2045,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
@@ -2068,7 +2080,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -2103,7 +2115,7 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
@@ -2138,7 +2150,7 @@
         <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -2173,7 +2185,7 @@
         <v>33</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -2208,7 +2220,7 @@
         <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -2243,7 +2255,7 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -2278,7 +2290,7 @@
         <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -2313,7 +2325,7 @@
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -2348,7 +2360,7 @@
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -2383,7 +2395,7 @@
         <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -2558,7 +2570,7 @@
         <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -2593,7 +2605,7 @@
         <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
@@ -2628,7 +2640,7 @@
         <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -2663,7 +2675,7 @@
         <v>11</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -2698,7 +2710,7 @@
         <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -2733,7 +2745,7 @@
         <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -2768,7 +2780,7 @@
         <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -2803,7 +2815,7 @@
         <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -2838,7 +2850,7 @@
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -2873,7 +2885,7 @@
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -2908,7 +2920,7 @@
         <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -2943,7 +2955,7 @@
         <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -2978,7 +2990,7 @@
         <v>21</v>
       </c>
       <c r="D56" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
@@ -3013,7 +3025,7 @@
         <v>21</v>
       </c>
       <c r="D57" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E57" t="b">
         <v>0</v>
@@ -3048,7 +3060,7 @@
         <v>21</v>
       </c>
       <c r="D58" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E58" t="b">
         <v>0</v>
@@ -3083,7 +3095,7 @@
         <v>21</v>
       </c>
       <c r="D59" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -3118,7 +3130,7 @@
         <v>17</v>
       </c>
       <c r="D60" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
@@ -3153,7 +3165,7 @@
         <v>17</v>
       </c>
       <c r="D61" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -3188,7 +3200,7 @@
         <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
@@ -3223,7 +3235,7 @@
         <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
@@ -3258,7 +3270,7 @@
         <v>23</v>
       </c>
       <c r="D64" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E64" t="b">
         <v>0</v>
@@ -3293,7 +3305,7 @@
         <v>23</v>
       </c>
       <c r="D65" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -3328,7 +3340,7 @@
         <v>23</v>
       </c>
       <c r="D66" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
@@ -3363,7 +3375,7 @@
         <v>23</v>
       </c>
       <c r="D67" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -3398,7 +3410,7 @@
         <v>19</v>
       </c>
       <c r="D68" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E68" t="b">
         <v>0</v>
@@ -3433,7 +3445,7 @@
         <v>19</v>
       </c>
       <c r="D69" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -3468,7 +3480,7 @@
         <v>19</v>
       </c>
       <c r="D70" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -3503,7 +3515,7 @@
         <v>19</v>
       </c>
       <c r="D71" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E71" t="b">
         <v>0</v>
@@ -3529,16 +3541,16 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B72" t="s">
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D72" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E72" t="b">
         <v>0</v>
@@ -3564,16 +3576,16 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B73" t="s">
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D73" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E73" t="b">
         <v>0</v>
@@ -3599,13 +3611,13 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B74" t="s">
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D74" t="s">
         <v>34</v>
@@ -3634,13 +3646,13 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D75" t="s">
         <v>35</v>
@@ -3669,16 +3681,16 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B76" t="s">
         <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D76" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E76" t="b">
         <v>0</v>
@@ -3704,16 +3716,16 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B77" t="s">
         <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D77" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E77" t="b">
         <v>0</v>
@@ -3739,16 +3751,16 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B78" t="s">
         <v>8</v>
       </c>
       <c r="C78" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D78" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E78" t="b">
         <v>0</v>
@@ -3774,16 +3786,16 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D79" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E79" t="b">
         <v>0</v>
@@ -3809,13 +3821,13 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D80" t="s">
         <v>34</v>
@@ -3844,13 +3856,13 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B81" t="s">
         <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D81" t="s">
         <v>35</v>
@@ -3879,16 +3891,16 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B82" t="s">
         <v>8</v>
       </c>
       <c r="C82" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D82" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E82" t="b">
         <v>0</v>
@@ -3914,16 +3926,16 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D83" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E83" t="b">
         <v>0</v>
@@ -3947,8 +3959,78 @@
         <v>1</v>
       </c>
     </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" t="s">
+        <v>50</v>
+      </c>
+      <c r="E84" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84" t="b">
+        <v>1</v>
+      </c>
+      <c r="H84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+      <c r="J84" t="b">
+        <v>1</v>
+      </c>
+      <c r="K84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E85" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+      <c r="G85" t="b">
+        <v>1</v>
+      </c>
+      <c r="H85" t="b">
+        <v>1</v>
+      </c>
+      <c r="I85" t="b">
+        <v>1</v>
+      </c>
+      <c r="J85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K85" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K83" xr:uid="{549ABC9E-401F-4507-8765-75A12C3B174F}"/>
+  <autoFilter ref="A1:K85" xr:uid="{549ABC9E-401F-4507-8765-75A12C3B174F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
labelling dictionary and fixing for HTI's case
</commit_message>
<xml_diff>
--- a/input_tool/edu_analysistools_loa.xlsx
+++ b/input_tool/edu_analysistools_loa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann SAY\Desktop\git\EduAnalysisTool\input_tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/EduAnalysisTool/input_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7276E6A8-92F6-4252-B86D-19E267DE1BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7276E6A8-92F6-4252-B86D-19E267DE1BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C4594ED-033C-4388-8024-9B4F927F4DF9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{172E695D-8722-4AF3-920F-94814F3A8B09}"/>
+    <workbookView xWindow="-19290" yWindow="-3720" windowWidth="19380" windowHeight="11460" xr2:uid="{172E695D-8722-4AF3-920F-94814F3A8B09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -155,12 +155,6 @@
     <t>edu_ind_no_access_d</t>
   </si>
   <si>
-    <t>pop_group</t>
-  </si>
-  <si>
-    <t>pop_group, ind_gender</t>
-  </si>
-  <si>
     <t>overall</t>
   </si>
   <si>
@@ -191,16 +185,22 @@
     <t>% of children accessing another type of education?</t>
   </si>
   <si>
-    <t>edu_school_cycle_d, pop_group</t>
-  </si>
-  <si>
-    <t>edu_school_cycle_d, pop_group, ind_gender</t>
-  </si>
-  <si>
-    <t>edu_school_cycle_d,pop_group</t>
-  </si>
-  <si>
-    <t>edu_school_cycle_d,pop_group, ind_gender</t>
+    <t>setting</t>
+  </si>
+  <si>
+    <t>setting, ind_gender</t>
+  </si>
+  <si>
+    <t>edu_school_cycle_d, setting</t>
+  </si>
+  <si>
+    <t>edu_school_cycle_d, setting, ind_gender</t>
+  </si>
+  <si>
+    <t>edu_school_cycle_d,setting</t>
+  </si>
+  <si>
+    <t>edu_school_cycle_d,setting, ind_gender</t>
   </si>
 </sst>
 </file>
@@ -1044,17 +1044,17 @@
   <dimension ref="A1:K85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.77734375" customWidth="1"/>
-    <col min="2" max="4" width="36.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="61.7109375" customWidth="1"/>
+    <col min="2" max="4" width="36.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1068,13 +1068,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>44</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -1086,10 +1086,10 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -1159,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1194,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -1229,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -1264,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -1299,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -1369,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -1439,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
@@ -1824,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
@@ -1894,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -1929,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -1964,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
@@ -1999,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -2034,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
@@ -2069,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -2104,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
@@ -2139,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -2174,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>33</v>
       </c>
       <c r="D33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -2209,7 +2209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -2244,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -2279,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -2349,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -2384,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>20</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>17</v>
       </c>
       <c r="D60" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
@@ -3154,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>17</v>
       </c>
       <c r="D61" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -3189,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
@@ -3224,7 +3224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
@@ -3259,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>22</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>23</v>
       </c>
       <c r="D64" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E64" t="b">
         <v>0</v>
@@ -3294,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>22</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>23</v>
       </c>
       <c r="D65" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -3329,7 +3329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>22</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>23</v>
       </c>
       <c r="D66" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
@@ -3364,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>22</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>23</v>
       </c>
       <c r="D67" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -3399,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>19</v>
       </c>
       <c r="D68" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E68" t="b">
         <v>0</v>
@@ -3434,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>19</v>
       </c>
       <c r="D69" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -3469,7 +3469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>19</v>
       </c>
       <c r="D70" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -3504,7 +3504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -3515,78 +3515,78 @@
         <v>19</v>
       </c>
       <c r="D71" t="s">
+        <v>49</v>
+      </c>
+      <c r="E71" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" t="b">
+        <v>0</v>
+      </c>
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+      <c r="J71" t="b">
+        <v>1</v>
+      </c>
+      <c r="K71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>44</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" t="s">
+        <v>47</v>
+      </c>
+      <c r="D72" t="s">
+        <v>38</v>
+      </c>
+      <c r="E72" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+      <c r="J72" t="b">
+        <v>0</v>
+      </c>
+      <c r="K72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>47</v>
+      </c>
+      <c r="D73" t="s">
         <v>39</v>
       </c>
-      <c r="E71" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" t="b">
-        <v>0</v>
-      </c>
-      <c r="G71" t="b">
-        <v>0</v>
-      </c>
-      <c r="H71" t="b">
-        <v>0</v>
-      </c>
-      <c r="I71" t="b">
-        <v>0</v>
-      </c>
-      <c r="J71" t="b">
-        <v>1</v>
-      </c>
-      <c r="K71" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>46</v>
-      </c>
-      <c r="B72" t="s">
-        <v>8</v>
-      </c>
-      <c r="C72" t="s">
-        <v>49</v>
-      </c>
-      <c r="D72" t="s">
-        <v>40</v>
-      </c>
-      <c r="E72" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" t="b">
-        <v>0</v>
-      </c>
-      <c r="G72" t="b">
-        <v>0</v>
-      </c>
-      <c r="H72" t="b">
-        <v>0</v>
-      </c>
-      <c r="I72" t="b">
-        <v>0</v>
-      </c>
-      <c r="J72" t="b">
-        <v>0</v>
-      </c>
-      <c r="K72" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>46</v>
-      </c>
-      <c r="B73" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" t="s">
-        <v>49</v>
-      </c>
-      <c r="D73" t="s">
-        <v>41</v>
-      </c>
       <c r="E73" t="b">
         <v>0</v>
       </c>
@@ -3609,15 +3609,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B74" t="s">
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D74" t="s">
         <v>34</v>
@@ -3644,15 +3644,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D75" t="s">
         <v>35</v>
@@ -3679,124 +3679,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>44</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" t="s">
+        <v>48</v>
+      </c>
+      <c r="E76" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" t="b">
+        <v>0</v>
+      </c>
+      <c r="I76" t="b">
+        <v>0</v>
+      </c>
+      <c r="J76" t="b">
+        <v>0</v>
+      </c>
+      <c r="K76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>44</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>47</v>
+      </c>
+      <c r="D77" t="s">
+        <v>49</v>
+      </c>
+      <c r="E77" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H77" t="b">
+        <v>0</v>
+      </c>
+      <c r="I77" t="b">
+        <v>0</v>
+      </c>
+      <c r="J77" t="b">
+        <v>0</v>
+      </c>
+      <c r="K77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>45</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
         <v>46</v>
       </c>
-      <c r="B76" t="s">
-        <v>8</v>
-      </c>
-      <c r="C76" t="s">
-        <v>49</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="D78" t="s">
         <v>38</v>
       </c>
-      <c r="E76" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" t="b">
-        <v>0</v>
-      </c>
-      <c r="G76" t="b">
-        <v>0</v>
-      </c>
-      <c r="H76" t="b">
-        <v>0</v>
-      </c>
-      <c r="I76" t="b">
-        <v>0</v>
-      </c>
-      <c r="J76" t="b">
-        <v>0</v>
-      </c>
-      <c r="K76" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="E78" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" t="b">
+        <v>0</v>
+      </c>
+      <c r="J78" t="b">
+        <v>0</v>
+      </c>
+      <c r="K78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>45</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
         <v>46</v>
       </c>
-      <c r="B77" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" t="s">
-        <v>49</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="D79" t="s">
         <v>39</v>
       </c>
-      <c r="E77" t="b">
-        <v>0</v>
-      </c>
-      <c r="F77" t="b">
-        <v>0</v>
-      </c>
-      <c r="G77" t="b">
-        <v>0</v>
-      </c>
-      <c r="H77" t="b">
-        <v>0</v>
-      </c>
-      <c r="I77" t="b">
-        <v>0</v>
-      </c>
-      <c r="J77" t="b">
-        <v>0</v>
-      </c>
-      <c r="K77" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>47</v>
-      </c>
-      <c r="B78" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" t="s">
-        <v>48</v>
-      </c>
-      <c r="D78" t="s">
-        <v>40</v>
-      </c>
-      <c r="E78" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" t="b">
-        <v>0</v>
-      </c>
-      <c r="G78" t="b">
-        <v>0</v>
-      </c>
-      <c r="H78" t="b">
-        <v>0</v>
-      </c>
-      <c r="I78" t="b">
-        <v>0</v>
-      </c>
-      <c r="J78" t="b">
-        <v>0</v>
-      </c>
-      <c r="K78" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>47</v>
-      </c>
-      <c r="B79" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" t="s">
-        <v>48</v>
-      </c>
-      <c r="D79" t="s">
-        <v>41</v>
-      </c>
       <c r="E79" t="b">
         <v>0</v>
       </c>
@@ -3819,15 +3819,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D80" t="s">
         <v>34</v>
@@ -3854,15 +3854,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B81" t="s">
         <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D81" t="s">
         <v>35</v>
@@ -3889,19 +3889,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B82" t="s">
         <v>8</v>
       </c>
       <c r="C82" t="s">
+        <v>46</v>
+      </c>
+      <c r="D82" t="s">
         <v>48</v>
       </c>
-      <c r="D82" t="s">
-        <v>38</v>
-      </c>
       <c r="E82" t="b">
         <v>0</v>
       </c>
@@ -3924,18 +3924,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D83" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E83" t="b">
         <v>0</v>
@@ -3959,7 +3959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
fixing labelling, source instead of function
</commit_message>
<xml_diff>
--- a/input_tool/edu_analysistools_loa.xlsx
+++ b/input_tool/edu_analysistools_loa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/EduAnalysisTool/input_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{C3CB7579-362D-4DB3-A6E6-0B702A8819F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFF32CC4-B5D0-464C-BE87-3DBAB47535E1}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{C3CB7579-362D-4DB3-A6E6-0B702A8819F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5B9740C-5924-4E54-B094-545CD936DFFF}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{172E695D-8722-4AF3-920F-94814F3A8B09}"/>
+    <workbookView xWindow="-19290" yWindow="-3720" windowWidth="19380" windowHeight="11460" xr2:uid="{172E695D-8722-4AF3-920F-94814F3A8B09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>edu_school_cycle_d</t>
   </si>
   <si>
-    <t>edu_school_cycle_d, ind_gender</t>
-  </si>
-  <si>
     <t>% children 5 to 18 y.o. who did not attended school or any early childhood education program at any time during the 2023-2024 school year</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>overall</t>
   </si>
   <si>
-    <t>overall, ind_gender</t>
-  </si>
-  <si>
     <t>access</t>
   </si>
   <si>
@@ -182,25 +176,31 @@
     <t>setting</t>
   </si>
   <si>
-    <t>setting, ind_gender</t>
-  </si>
-  <si>
     <t>edu_school_cycle_d, setting</t>
   </si>
   <si>
-    <t>edu_school_cycle_d, setting, ind_gender</t>
-  </si>
-  <si>
     <t>edu_school_cycle_d,setting</t>
   </si>
   <si>
-    <t>edu_school_cycle_d,setting, ind_gender</t>
-  </si>
-  <si>
     <t>% of children one year before primary school entry age attending early childhood education or primary school.</t>
   </si>
   <si>
     <t>% of children one year before primary school entry age attending primary school.</t>
+  </si>
+  <si>
+    <t>overall, child_gender_d</t>
+  </si>
+  <si>
+    <t>edu_school_cycle_d, child_gender_d</t>
+  </si>
+  <si>
+    <t>setting, child_gender_d</t>
+  </si>
+  <si>
+    <t>edu_school_cycle_d, setting, child_gender_d</t>
+  </si>
+  <si>
+    <t>edu_school_cycle_d,setting, child_gender_d</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1049,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE1FF5D-95CC-49D0-8C54-8D9CF98199B7}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
       <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
@@ -1078,13 +1077,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
         <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -1096,10 +1095,10 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1110,7 +1109,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1134,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -1169,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1180,7 +1179,7 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1204,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1215,7 +1214,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -1239,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -1274,7 +1273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1285,7 +1284,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -1309,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1320,7 +1319,7 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -1344,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -1379,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1390,7 +1389,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -1414,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1425,7 +1424,7 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -1449,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1554,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1589,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1624,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1635,7 +1634,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
@@ -1659,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1670,7 +1669,7 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E18" t="b">
         <v>1</v>
@@ -1694,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
@@ -1729,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1740,7 +1739,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E20" t="b">
         <v>1</v>
@@ -1764,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1775,7 +1774,7 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E21" t="b">
         <v>1</v>
@@ -1799,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1810,7 +1809,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
@@ -1834,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1845,7 +1844,7 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
@@ -1869,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1880,7 +1879,7 @@
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
@@ -1904,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1915,7 +1914,7 @@
         <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -1939,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1950,7 +1949,7 @@
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -1974,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1985,7 +1984,7 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
@@ -2009,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2020,7 +2019,7 @@
         <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -2044,7 +2043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2055,7 +2054,7 @@
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
@@ -2079,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2090,7 +2089,7 @@
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -2114,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -2125,7 +2124,7 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
@@ -2149,19 +2148,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
         <v>35</v>
       </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" t="s">
-        <v>36</v>
-      </c>
       <c r="E32" t="b">
         <v>0</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -2195,7 +2194,7 @@
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -2219,18 +2218,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -2254,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -2265,7 +2264,7 @@
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -2289,18 +2288,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -2324,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -2335,7 +2334,7 @@
         <v>31</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -2359,18 +2358,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -2394,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -2405,7 +2404,7 @@
         <v>31</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -2429,15 +2428,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" t="s">
         <v>32</v>
@@ -2464,7 +2463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -2499,18 +2498,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -2534,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -2545,7 +2544,7 @@
         <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -2569,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2577,7 +2576,7 @@
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D44" t="s">
         <v>32</v>
@@ -2604,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -2612,10 +2611,10 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D45" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
@@ -2639,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2647,10 +2646,10 @@
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -2674,7 +2673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2682,11 +2681,11 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" t="s">
         <v>52</v>
       </c>
-      <c r="D47" t="s">
-        <v>49</v>
-      </c>
       <c r="E47" t="b">
         <v>0</v>
       </c>
@@ -2709,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -2717,7 +2716,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D48" t="s">
         <v>32</v>
@@ -2744,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.75">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -2752,10 +2751,10 @@
         <v>8</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -2779,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -2787,10 +2786,10 @@
         <v>8</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -2814,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.75">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -2822,10 +2821,10 @@
         <v>8</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -2849,7 +2848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -2884,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -2895,7 +2894,7 @@
         <v>13</v>
       </c>
       <c r="D53" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -2919,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -2930,7 +2929,7 @@
         <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -2954,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -2965,7 +2964,7 @@
         <v>13</v>
       </c>
       <c r="D55" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -3035,7 +3034,7 @@
         <v>19</v>
       </c>
       <c r="D57" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E57" t="b">
         <v>0</v>
@@ -3070,7 +3069,7 @@
         <v>19</v>
       </c>
       <c r="D58" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E58" t="b">
         <v>0</v>
@@ -3105,7 +3104,7 @@
         <v>19</v>
       </c>
       <c r="D59" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -3129,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -3164,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3175,7 +3174,7 @@
         <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -3199,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3210,7 +3209,7 @@
         <v>15</v>
       </c>
       <c r="D62" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
@@ -3234,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3245,7 +3244,7 @@
         <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
@@ -3315,7 +3314,7 @@
         <v>21</v>
       </c>
       <c r="D65" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -3350,7 +3349,7 @@
         <v>21</v>
       </c>
       <c r="D66" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
@@ -3385,7 +3384,7 @@
         <v>21</v>
       </c>
       <c r="D67" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -3409,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -3444,7 +3443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -3455,7 +3454,7 @@
         <v>17</v>
       </c>
       <c r="D69" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -3479,7 +3478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -3490,7 +3489,7 @@
         <v>17</v>
       </c>
       <c r="D70" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -3514,7 +3513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -3525,7 +3524,7 @@
         <v>17</v>
       </c>
       <c r="D71" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E71" t="b">
         <v>0</v>
@@ -3549,18 +3548,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A72" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B72" t="s">
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D72" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E72" t="b">
         <v>0</v>
@@ -3584,18 +3583,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A73" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B73" t="s">
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D73" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E73" t="b">
         <v>0</v>
@@ -3619,15 +3618,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A74" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B74" t="s">
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D74" t="s">
         <v>32</v>
@@ -3654,190 +3653,190 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A75" t="s">
+        <v>40</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75" t="b">
+        <v>0</v>
+      </c>
+      <c r="I75" t="b">
+        <v>0</v>
+      </c>
+      <c r="J75" t="b">
+        <v>0</v>
+      </c>
+      <c r="K75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A76" t="s">
+        <v>40</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76" t="s">
+        <v>44</v>
+      </c>
+      <c r="E76" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" t="b">
+        <v>0</v>
+      </c>
+      <c r="I76" t="b">
+        <v>0</v>
+      </c>
+      <c r="J76" t="b">
+        <v>0</v>
+      </c>
+      <c r="K76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A77" t="s">
+        <v>40</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>43</v>
+      </c>
+      <c r="D77" t="s">
+        <v>51</v>
+      </c>
+      <c r="E77" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H77" t="b">
+        <v>0</v>
+      </c>
+      <c r="I77" t="b">
+        <v>0</v>
+      </c>
+      <c r="J77" t="b">
+        <v>0</v>
+      </c>
+      <c r="K77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A78" t="s">
+        <v>41</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
         <v>42</v>
       </c>
-      <c r="B75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C75" t="s">
-        <v>45</v>
-      </c>
-      <c r="D75" t="s">
-        <v>33</v>
-      </c>
-      <c r="E75" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" t="b">
-        <v>0</v>
-      </c>
-      <c r="G75" t="b">
-        <v>0</v>
-      </c>
-      <c r="H75" t="b">
-        <v>0</v>
-      </c>
-      <c r="I75" t="b">
-        <v>0</v>
-      </c>
-      <c r="J75" t="b">
-        <v>0</v>
-      </c>
-      <c r="K75" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
-      <c r="A76" t="s">
+      <c r="D78" t="s">
+        <v>35</v>
+      </c>
+      <c r="E78" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" t="b">
+        <v>0</v>
+      </c>
+      <c r="J78" t="b">
+        <v>0</v>
+      </c>
+      <c r="K78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A79" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
         <v>42</v>
       </c>
-      <c r="B76" t="s">
-        <v>8</v>
-      </c>
-      <c r="C76" t="s">
-        <v>45</v>
-      </c>
-      <c r="D76" t="s">
-        <v>46</v>
-      </c>
-      <c r="E76" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" t="b">
-        <v>0</v>
-      </c>
-      <c r="G76" t="b">
-        <v>0</v>
-      </c>
-      <c r="H76" t="b">
-        <v>0</v>
-      </c>
-      <c r="I76" t="b">
-        <v>0</v>
-      </c>
-      <c r="J76" t="b">
-        <v>0</v>
-      </c>
-      <c r="K76" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
-      <c r="A77" t="s">
+      <c r="D79" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
+      </c>
+      <c r="H79" t="b">
+        <v>0</v>
+      </c>
+      <c r="I79" t="b">
+        <v>0</v>
+      </c>
+      <c r="J79" t="b">
+        <v>0</v>
+      </c>
+      <c r="K79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A80" t="s">
+        <v>41</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
         <v>42</v>
-      </c>
-      <c r="B77" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" t="s">
-        <v>45</v>
-      </c>
-      <c r="D77" t="s">
-        <v>47</v>
-      </c>
-      <c r="E77" t="b">
-        <v>0</v>
-      </c>
-      <c r="F77" t="b">
-        <v>0</v>
-      </c>
-      <c r="G77" t="b">
-        <v>0</v>
-      </c>
-      <c r="H77" t="b">
-        <v>0</v>
-      </c>
-      <c r="I77" t="b">
-        <v>0</v>
-      </c>
-      <c r="J77" t="b">
-        <v>0</v>
-      </c>
-      <c r="K77" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
-      <c r="A78" t="s">
-        <v>43</v>
-      </c>
-      <c r="B78" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" t="s">
-        <v>44</v>
-      </c>
-      <c r="D78" t="s">
-        <v>36</v>
-      </c>
-      <c r="E78" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" t="b">
-        <v>0</v>
-      </c>
-      <c r="G78" t="b">
-        <v>0</v>
-      </c>
-      <c r="H78" t="b">
-        <v>0</v>
-      </c>
-      <c r="I78" t="b">
-        <v>0</v>
-      </c>
-      <c r="J78" t="b">
-        <v>0</v>
-      </c>
-      <c r="K78" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
-      <c r="A79" t="s">
-        <v>43</v>
-      </c>
-      <c r="B79" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" t="s">
-        <v>44</v>
-      </c>
-      <c r="D79" t="s">
-        <v>37</v>
-      </c>
-      <c r="E79" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" t="b">
-        <v>0</v>
-      </c>
-      <c r="G79" t="b">
-        <v>0</v>
-      </c>
-      <c r="H79" t="b">
-        <v>0</v>
-      </c>
-      <c r="I79" t="b">
-        <v>0</v>
-      </c>
-      <c r="J79" t="b">
-        <v>0</v>
-      </c>
-      <c r="K79" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
-      <c r="A80" t="s">
-        <v>43</v>
-      </c>
-      <c r="B80" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" t="s">
-        <v>44</v>
       </c>
       <c r="D80" t="s">
         <v>32</v>
@@ -3864,54 +3863,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A81" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
         <v>8</v>
       </c>
       <c r="C81" t="s">
+        <v>42</v>
+      </c>
+      <c r="D81" t="s">
+        <v>50</v>
+      </c>
+      <c r="E81" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+      <c r="H81" t="b">
+        <v>0</v>
+      </c>
+      <c r="I81" t="b">
+        <v>0</v>
+      </c>
+      <c r="J81" t="b">
+        <v>0</v>
+      </c>
+      <c r="K81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A82" t="s">
+        <v>41</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82" t="s">
         <v>44</v>
       </c>
-      <c r="D81" t="s">
-        <v>33</v>
-      </c>
-      <c r="E81" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" t="b">
-        <v>0</v>
-      </c>
-      <c r="G81" t="b">
-        <v>0</v>
-      </c>
-      <c r="H81" t="b">
-        <v>0</v>
-      </c>
-      <c r="I81" t="b">
-        <v>0</v>
-      </c>
-      <c r="J81" t="b">
-        <v>0</v>
-      </c>
-      <c r="K81" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
-      <c r="A82" t="s">
-        <v>43</v>
-      </c>
-      <c r="B82" t="s">
-        <v>8</v>
-      </c>
-      <c r="C82" t="s">
-        <v>44</v>
-      </c>
-      <c r="D82" t="s">
-        <v>46</v>
-      </c>
       <c r="E82" t="b">
         <v>0</v>
       </c>
@@ -3934,18 +3933,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D83" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E83" t="b">
         <v>0</v>
@@ -3969,7 +3968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -3980,7 +3979,7 @@
         <v>9</v>
       </c>
       <c r="D84" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E84" t="b">
         <v>0</v>
@@ -4004,7 +4003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -4015,7 +4014,7 @@
         <v>9</v>
       </c>
       <c r="D85" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E85" t="b">
         <v>0</v>
@@ -4040,14 +4039,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K85" xr:uid="{EFE1FF5D-95CC-49D0-8C54-8D9CF98199B7}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="edu_level1_overage_learners_d"/>
-        <filter val="edu_level2_overage_learners_d"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K85" xr:uid="{EFE1FF5D-95CC-49D0-8C54-8D9CF98199B7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>